<commit_message>
Prepare for regression testing/ updated all the past test case to match latest change of requirements
</commit_message>
<xml_diff>
--- a/testing/iteration 4/testcase (iter 4).xlsx
+++ b/testing/iteration 4/testcase (iter 4).xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Boyofthefuture\Documents\NetBeansProjects\is203_g3t3\testing\iteration 4\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="11835" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19420" windowHeight="11840" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="TestPlan" sheetId="6" r:id="rId1"/>
@@ -902,26 +897,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -945,6 +922,24 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="50">
     <cellStyle name="Calculation" xfId="15" builtinId="22"/>
@@ -1339,19 +1334,19 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="82.125" customWidth="1"/>
-    <col min="2" max="2" width="49.375" customWidth="1"/>
+    <col min="1" max="1" width="82.08203125" customWidth="1"/>
+    <col min="2" max="2" width="49.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="27.75" x14ac:dyDescent="0.4">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:2" ht="28" x14ac:dyDescent="0.6">
+      <c r="A1" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="20"/>
-    </row>
-    <row r="2" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B1" s="29"/>
+    </row>
+    <row r="2" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="9" t="s">
         <v>69</v>
       </c>
@@ -1359,7 +1354,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="47" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="9" t="s">
         <v>70</v>
       </c>
@@ -1367,7 +1362,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="9" t="s">
         <v>77</v>
       </c>
@@ -1375,7 +1370,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="9" t="s">
         <v>76</v>
       </c>
@@ -1383,7 +1378,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="9" t="s">
         <v>75</v>
       </c>
@@ -1413,25 +1408,25 @@
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="38.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.58203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="48" customWidth="1"/>
     <col min="4" max="4" width="18.5" customWidth="1"/>
     <col min="5" max="5" width="25" customWidth="1"/>
-    <col min="6" max="6" width="35.875" customWidth="1"/>
-    <col min="7" max="7" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.83203125" customWidth="1"/>
+    <col min="7" max="7" width="12.58203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
       <c r="G1" s="19" t="s">
         <v>117</v>
       </c>
@@ -1439,7 +1434,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1471,7 +1466,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1503,7 +1498,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="141.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="139.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -1535,7 +1530,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="93" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -1567,7 +1562,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="173.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="170.5" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -1599,7 +1594,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="157.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="139.5" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -1631,7 +1626,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="108.5" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -1663,7 +1658,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1693,19 +1688,19 @@
       <selection activeCell="I2" sqref="I2:J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.625" customWidth="1"/>
+    <col min="1" max="1" width="7.58203125" customWidth="1"/>
     <col min="2" max="2" width="39" customWidth="1"/>
-    <col min="3" max="3" width="46.875" customWidth="1"/>
-    <col min="4" max="4" width="16.875" customWidth="1"/>
-    <col min="5" max="5" width="17.125" customWidth="1"/>
-    <col min="6" max="6" width="78.375" customWidth="1"/>
-    <col min="7" max="7" width="12.375" customWidth="1"/>
+    <col min="3" max="3" width="46.83203125" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" customWidth="1"/>
+    <col min="5" max="5" width="17.08203125" customWidth="1"/>
+    <col min="6" max="6" width="78.33203125" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" customWidth="1"/>
     <col min="9" max="9" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="G1" t="s">
         <v>117</v>
       </c>
@@ -1713,7 +1708,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
@@ -1745,7 +1740,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="11">
         <v>1</v>
       </c>
@@ -1777,7 +1772,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="11">
         <v>2</v>
       </c>
@@ -1809,7 +1804,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11">
         <v>3</v>
       </c>
@@ -1841,7 +1836,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="11">
         <v>4</v>
       </c>
@@ -1873,7 +1868,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="11">
         <v>5</v>
       </c>
@@ -1924,28 +1919,28 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.375" style="5" customWidth="1"/>
-    <col min="2" max="2" width="28.375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="36.625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="36.58203125" style="5" customWidth="1"/>
     <col min="4" max="4" width="40.5" style="5" customWidth="1"/>
-    <col min="5" max="5" width="33.375" style="5" customWidth="1"/>
-    <col min="6" max="6" width="25.625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="12.125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="8.625" style="5"/>
-    <col min="9" max="9" width="10.125" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.625" style="5"/>
+    <col min="5" max="5" width="33.33203125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="25.58203125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="12.08203125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="8.58203125" style="5"/>
+    <col min="9" max="9" width="10.08203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.58203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
       <c r="G1" s="5" t="s">
         <v>117</v>
       </c>
@@ -1953,7 +1948,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="3" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1985,7 +1980,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="63" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="62" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -2017,7 +2012,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -2049,7 +2044,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -2081,7 +2076,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -2113,7 +2108,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -2142,7 +2137,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -2174,7 +2169,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -2206,7 +2201,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -2238,7 +2233,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -2270,7 +2265,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -2302,7 +2297,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>11</v>
       </c>
@@ -2334,7 +2329,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -2366,7 +2361,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>13</v>
       </c>
@@ -2398,7 +2393,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="15" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" s="15" customFormat="1" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A16" s="15">
         <v>14</v>
       </c>
@@ -2452,32 +2447,32 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.625" style="1"/>
-    <col min="2" max="2" width="48.125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.58203125" style="1"/>
+    <col min="2" max="2" width="48.08203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.08203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.58203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="20" style="1" customWidth="1"/>
     <col min="7" max="7" width="16.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.625" style="1"/>
+    <col min="8" max="16384" width="8.58203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
       <c r="F1" s="7"/>
       <c r="G1" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -2503,7 +2498,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="93" x14ac:dyDescent="0.35">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -2525,7 +2520,7 @@
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
     </row>
-    <row r="4" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="93" x14ac:dyDescent="0.35">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -2547,9 +2542,9 @@
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
     </row>
-    <row r="5" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="108.5" x14ac:dyDescent="0.35">
       <c r="A5" s="7"/>
-      <c r="B5" s="24"/>
+      <c r="B5" s="20"/>
       <c r="C5" s="8" t="s">
         <v>67</v>
       </c>
@@ -2559,7 +2554,7 @@
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -2567,7 +2562,7 @@
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -2575,7 +2570,7 @@
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -2583,7 +2578,7 @@
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -2591,7 +2586,7 @@
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -2599,7 +2594,7 @@
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -2607,7 +2602,7 @@
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -2637,269 +2632,269 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.125" style="34" customWidth="1"/>
-    <col min="2" max="2" width="20.875" style="34" customWidth="1"/>
-    <col min="3" max="3" width="41.125" style="34" customWidth="1"/>
-    <col min="4" max="4" width="38" style="34" customWidth="1"/>
-    <col min="5" max="6" width="20.625" style="34" customWidth="1"/>
-    <col min="7" max="7" width="26.875" style="34" customWidth="1"/>
-    <col min="8" max="8" width="20.625" style="34" customWidth="1"/>
-    <col min="9" max="9" width="23.125" style="13" customWidth="1"/>
-    <col min="10" max="16384" width="8.875" style="13"/>
+    <col min="1" max="1" width="6.08203125" style="28" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" style="28" customWidth="1"/>
+    <col min="3" max="3" width="41.08203125" style="28" customWidth="1"/>
+    <col min="4" max="4" width="38" style="28" customWidth="1"/>
+    <col min="5" max="6" width="20.58203125" style="28" customWidth="1"/>
+    <col min="7" max="7" width="26.83203125" style="28" customWidth="1"/>
+    <col min="8" max="8" width="20.58203125" style="28" customWidth="1"/>
+    <col min="9" max="9" width="23.08203125" style="13" customWidth="1"/>
+    <col min="10" max="16384" width="8.83203125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="33" t="s">
         <v>133</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
       <c r="I1" s="13" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="32" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="27" t="s">
+    <row r="2" spans="1:9" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="G2" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="H2" s="27" t="s">
+      <c r="H2" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="32" t="s">
+      <c r="I2" s="26" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="32" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28">
+    <row r="3" spans="1:9" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="22">
         <v>1</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="24" t="s">
         <v>135</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="G3" s="24" t="s">
         <v>135</v>
       </c>
-      <c r="H3" s="30" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" s="32" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="28">
+      <c r="H3" s="24" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="26" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="22">
         <v>2</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="24" t="s">
         <v>137</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="E4" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="F4" s="28" t="s">
+      <c r="F4" s="22" t="s">
         <v>139</v>
       </c>
-      <c r="G4" s="28" t="s">
+      <c r="G4" s="22" t="s">
         <v>139</v>
       </c>
-      <c r="H4" s="30" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="32" customFormat="1" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="28">
+      <c r="H4" s="24" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="26" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="22">
         <v>3</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="22" t="s">
         <v>140</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="24" t="s">
         <v>141</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="F5" s="28" t="s">
+      <c r="F5" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="G5" s="28" t="s">
+      <c r="G5" s="22" t="s">
         <v>144</v>
       </c>
-      <c r="H5" s="30" t="s">
+      <c r="H5" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="I5" s="33"/>
-    </row>
-    <row r="6" spans="1:9" s="32" customFormat="1" ht="87.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="28">
+      <c r="I5" s="27"/>
+    </row>
+    <row r="6" spans="1:9" s="26" customFormat="1" ht="88" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="22">
         <v>4</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="E6" s="28" t="s">
+      <c r="E6" s="22" t="s">
         <v>147</v>
       </c>
-      <c r="F6" s="31" t="s">
+      <c r="F6" s="25" t="s">
         <v>148</v>
       </c>
-      <c r="G6" s="28" t="s">
+      <c r="G6" s="22" t="s">
         <v>149</v>
       </c>
-      <c r="H6" s="28" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" s="32" customFormat="1" ht="126" x14ac:dyDescent="0.25">
-      <c r="A7" s="28">
+      <c r="H6" s="22" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="26" customFormat="1" ht="124" x14ac:dyDescent="0.35">
+      <c r="A7" s="22">
         <v>5</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="E7" s="28" t="s">
+      <c r="E7" s="22" t="s">
         <v>151</v>
       </c>
-      <c r="F7" s="31" t="s">
+      <c r="F7" s="25" t="s">
         <v>152</v>
       </c>
-      <c r="G7" s="28" t="s">
+      <c r="G7" s="22" t="s">
         <v>153</v>
       </c>
-      <c r="H7" s="28" t="s">
+      <c r="H7" s="22" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="32" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="28">
+    <row r="8" spans="1:9" s="26" customFormat="1" ht="108.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="22">
         <v>6</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="22" t="s">
         <v>154</v>
       </c>
-      <c r="D8" s="30" t="s">
+      <c r="D8" s="24" t="s">
         <v>155</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="F8" s="31" t="s">
+      <c r="F8" s="25" t="s">
         <v>157</v>
       </c>
-      <c r="G8" s="28" t="s">
+      <c r="G8" s="22" t="s">
         <v>158</v>
       </c>
-      <c r="H8" s="28" t="s">
+      <c r="H8" s="22" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="32" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="28">
+    <row r="9" spans="1:9" s="26" customFormat="1" ht="93" x14ac:dyDescent="0.35">
+      <c r="A9" s="22">
         <v>7</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="22" t="s">
         <v>159</v>
       </c>
-      <c r="D9" s="30" t="s">
+      <c r="D9" s="24" t="s">
         <v>160</v>
       </c>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="22" t="s">
         <v>161</v>
       </c>
-      <c r="F9" s="31" t="s">
+      <c r="F9" s="25" t="s">
         <v>162</v>
       </c>
-      <c r="G9" s="28" t="s">
+      <c r="G9" s="22" t="s">
         <v>163</v>
       </c>
-      <c r="H9" s="28" t="s">
+      <c r="H9" s="22" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="32" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="28">
+    <row r="10" spans="1:9" s="26" customFormat="1" ht="93" x14ac:dyDescent="0.35">
+      <c r="A10" s="22">
         <v>8</v>
       </c>
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="22" t="s">
         <v>164</v>
       </c>
-      <c r="D10" s="30" t="s">
+      <c r="D10" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="F10" s="31" t="s">
+      <c r="F10" s="25" t="s">
         <v>166</v>
       </c>
-      <c r="G10" s="28" t="s">
+      <c r="G10" s="22" t="s">
         <v>167</v>
       </c>
-      <c r="H10" s="28" t="s">
+      <c r="H10" s="22" t="s">
         <v>90</v>
       </c>
     </row>
@@ -2919,31 +2914,31 @@
       <selection activeCell="H4" sqref="G3:H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.625" style="5"/>
+    <col min="1" max="1" width="8.58203125" style="5"/>
     <col min="2" max="2" width="39.5" style="5" customWidth="1"/>
-    <col min="3" max="3" width="18.125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="13.875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="12.375" style="5" customWidth="1"/>
-    <col min="6" max="6" width="20.125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="13.125" style="5" customWidth="1"/>
-    <col min="8" max="16384" width="8.625" style="5"/>
+    <col min="3" max="3" width="18.08203125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="20.08203125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="13.08203125" style="5" customWidth="1"/>
+    <col min="8" max="16384" width="8.58203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
       <c r="G1" s="5" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="31" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -2970,7 +2965,7 @@
       </c>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -2988,7 +2983,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="157.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="155" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>2</v>
       </c>

</xml_diff>